<commit_message>
Implemented java document: comment  and Testng.Xml executable file
</commit_message>
<xml_diff>
--- a/Agrovet.Samadhan.Grader/testData/Book1.xlsx
+++ b/Agrovet.Samadhan.Grader/testData/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testing.engineer\git\Grader\Agrovet.Samadhan.Grader\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76321D8E-B5A4-4374-A1E6-56F54D162D8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556D0194-8F60-4CAE-A28B-D26C12FB1C0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23640" windowHeight="12930" xr2:uid="{F99DDD6B-DC0A-4C27-B8E5-578350DAA813}"/>
   </bookViews>
@@ -54,12 +54,6 @@
     <t>Emergency</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>fourthOtp</t>
   </si>
   <si>
@@ -112,6 +106,12 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>29</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +485,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -533,31 +533,31 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -573,7 +573,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -613,18 +613,18 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
         <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>